<commit_message>
menuFragement - OverlayService 기능 구현 완료
</commit_message>
<xml_diff>
--- a/문서/기획/Gaia 어플리케이션 설계-DB.xlsx
+++ b/문서/기획/Gaia 어플리케이션 설계-DB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ㄱㅎ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2017\WebMo\Gaia_Github3\문서\기획\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -298,10 +298,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2 : flowerNo이 1인 꽃이 2개 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>4 : flowerNo이 4인 꽃이 4개 있다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -471,6 +467,10 @@
   </si>
   <si>
     <t>꽃/스킬/업적 등의 번호(순서)는 [UI기획, 업적] 파일에 써 있는 순서입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2 : flowerNo이 2인 꽃이 2개 있다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1393,22 +1393,31 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1420,40 +1429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1465,127 +1441,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1659,6 +1515,150 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E1D1DD-D649-4562-9980-FF4DCC3509EE}">
   <dimension ref="B3:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1989,103 +1989,103 @@
   <sheetData>
     <row r="3" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="115"/>
-      <c r="N4" s="115"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="116"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="55"/>
     </row>
     <row r="6" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="71" t="s">
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="72"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="74" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
-      <c r="N7" s="124" t="s">
-        <v>119</v>
-      </c>
-      <c r="O7" s="125"/>
-      <c r="P7" s="125"/>
-      <c r="Q7" s="126"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="68"/>
+      <c r="N7" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="77"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="78"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="87"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="118">
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="70">
         <v>1</v>
       </c>
-      <c r="F8" s="119"/>
-      <c r="G8" s="120"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="72"/>
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="13"/>
-      <c r="N8" s="127"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="129"/>
+      <c r="N8" s="79"/>
+      <c r="O8" s="80"/>
+      <c r="P8" s="80"/>
+      <c r="Q8" s="81"/>
     </row>
     <row r="9" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="60"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="59" t="s">
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="62" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
       <c r="L9" s="16"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="131"/>
-      <c r="P9" s="131"/>
-      <c r="Q9" s="132"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="84"/>
     </row>
     <row r="10" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="121" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="122"/>
-      <c r="G10" s="123"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="73" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" s="15"/>
@@ -2093,108 +2093,108 @@
       <c r="L10" s="16"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="59" t="s">
+      <c r="C11" s="63"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="64"/>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="16"/>
-      <c r="N11" s="133" t="s">
-        <v>120</v>
-      </c>
-      <c r="O11" s="134"/>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="135"/>
+      <c r="N11" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="87"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="59" t="s">
+      <c r="B12" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="63"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="59" t="s">
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="82"/>
-      <c r="N12" s="136"/>
-      <c r="O12" s="137"/>
-      <c r="P12" s="137"/>
-      <c r="Q12" s="138"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="69"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="90"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="59" t="s">
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="60"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="59" t="s">
+      <c r="F13" s="63"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="82"/>
-      <c r="N13" s="136"/>
-      <c r="O13" s="137"/>
-      <c r="P13" s="137"/>
-      <c r="Q13" s="138"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="63"/>
+      <c r="K13" s="63"/>
+      <c r="L13" s="69"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="90"/>
     </row>
     <row r="14" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="60"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="92" t="s">
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="93"/>
-      <c r="G14" s="94"/>
-      <c r="H14" s="98" t="s">
+      <c r="F14" s="118"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="123" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="99"/>
-      <c r="J14" s="99"/>
-      <c r="K14" s="99"/>
-      <c r="L14" s="100"/>
-      <c r="N14" s="139"/>
-      <c r="O14" s="140"/>
-      <c r="P14" s="140"/>
-      <c r="Q14" s="141"/>
+      <c r="I14" s="124"/>
+      <c r="J14" s="124"/>
+      <c r="K14" s="124"/>
+      <c r="L14" s="125"/>
+      <c r="N14" s="91"/>
+      <c r="O14" s="92"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="93"/>
     </row>
     <row r="15" spans="2:17" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="95" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="96"/>
-      <c r="G15" s="97"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="122"/>
       <c r="H15" s="17"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
@@ -2203,30 +2203,30 @@
     </row>
     <row r="18" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="71" t="s">
+      <c r="B19" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="74" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="75"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="74" t="s">
+      <c r="F19" s="67"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="76"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="68"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="86" t="s">
+      <c r="B20" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="111"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="100"/>
       <c r="E20" s="6">
         <v>1</v>
       </c>
@@ -2236,18 +2236,18 @@
       <c r="G20" s="8">
         <v>3</v>
       </c>
-      <c r="H20" s="101"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="84"/>
-      <c r="L20" s="85"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
+      <c r="K20" s="113"/>
+      <c r="L20" s="126"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="60"/>
-      <c r="D21" s="109"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="43" t="s">
         <v>32</v>
       </c>
@@ -2257,20 +2257,20 @@
       <c r="G21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="59" t="s">
+      <c r="H21" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="82"/>
+      <c r="I21" s="63"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="69"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="109"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="43" t="s">
         <v>33</v>
       </c>
@@ -2280,20 +2280,20 @@
       <c r="G22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="59" t="s">
+      <c r="H22" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="82"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="69"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="60"/>
-      <c r="D23" s="109"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="43" t="s">
         <v>36</v>
       </c>
@@ -2303,20 +2303,20 @@
       <c r="G23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="59" t="s">
+      <c r="H23" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="82"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="69"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="60"/>
-      <c r="D24" s="109"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="43" t="s">
         <v>35</v>
       </c>
@@ -2326,20 +2326,20 @@
       <c r="G24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="59" t="s">
+      <c r="H24" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="82"/>
+      <c r="I24" s="63"/>
+      <c r="J24" s="63"/>
+      <c r="K24" s="63"/>
+      <c r="L24" s="69"/>
     </row>
     <row r="25" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="53" t="s">
+      <c r="B25" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="110"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="44" t="s">
         <v>35</v>
       </c>
@@ -2349,41 +2349,41 @@
       <c r="G25" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="H25" s="53" t="s">
+      <c r="H25" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="80"/>
+      <c r="I25" s="95"/>
+      <c r="J25" s="95"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="115"/>
     </row>
     <row r="30" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="71" t="s">
+      <c r="B31" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="72"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="71" t="s">
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="72"/>
-      <c r="G31" s="73"/>
-      <c r="H31" s="71" t="s">
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
-      <c r="K31" s="72"/>
-      <c r="L31" s="72"/>
-      <c r="M31" s="73"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="58"/>
     </row>
     <row r="32" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="112" t="s">
+      <c r="B32" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
+      <c r="C32" s="104"/>
+      <c r="D32" s="104"/>
       <c r="E32" s="20">
         <v>1</v>
       </c>
@@ -2393,19 +2393,19 @@
       <c r="G32" s="8">
         <v>3</v>
       </c>
-      <c r="H32" s="86"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="87"/>
-      <c r="K32" s="87"/>
-      <c r="L32" s="87"/>
-      <c r="M32" s="88"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="105"/>
     </row>
     <row r="33" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="107" t="s">
+      <c r="B33" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="108"/>
-      <c r="D33" s="108"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="102"/>
       <c r="E33" s="45" t="s">
         <v>57</v>
       </c>
@@ -2415,21 +2415,21 @@
       <c r="G33" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="H33" s="59" t="s">
+      <c r="H33" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="I33" s="60"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="60"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="82"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="63"/>
+      <c r="K33" s="63"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="69"/>
     </row>
     <row r="34" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="107" t="s">
+      <c r="B34" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="108"/>
-      <c r="D34" s="108"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="102"/>
       <c r="E34" s="45" t="s">
         <v>62</v>
       </c>
@@ -2439,21 +2439,21 @@
       <c r="G34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H34" s="59" t="s">
+      <c r="H34" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="60"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="82"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="69"/>
     </row>
     <row r="35" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="107" t="s">
+      <c r="B35" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="108"/>
-      <c r="D35" s="108"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
       <c r="E35" s="45" t="s">
         <v>60</v>
       </c>
@@ -2463,21 +2463,21 @@
       <c r="G35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H35" s="59" t="s">
+      <c r="H35" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="82"/>
+      <c r="I35" s="63"/>
+      <c r="J35" s="63"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="63"/>
+      <c r="M35" s="69"/>
     </row>
     <row r="36" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="108"/>
-      <c r="D36" s="108"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="102"/>
       <c r="E36" s="45" t="s">
         <v>65</v>
       </c>
@@ -2487,21 +2487,21 @@
       <c r="G36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H36" s="59" t="s">
+      <c r="H36" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="82"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
+      <c r="K36" s="63"/>
+      <c r="L36" s="63"/>
+      <c r="M36" s="69"/>
     </row>
     <row r="37" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="107" t="s">
+      <c r="B37" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="108"/>
-      <c r="D37" s="108"/>
+      <c r="C37" s="102"/>
+      <c r="D37" s="102"/>
       <c r="E37" s="45" t="s">
         <v>34</v>
       </c>
@@ -2511,21 +2511,21 @@
       <c r="G37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H37" s="59" t="s">
+      <c r="H37" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="I37" s="60"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="82"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="69"/>
     </row>
     <row r="38" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="107" t="s">
+      <c r="B38" s="101" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="108"/>
-      <c r="D38" s="108"/>
+      <c r="C38" s="102"/>
+      <c r="D38" s="102"/>
       <c r="E38" s="46" t="s">
         <v>35</v>
       </c>
@@ -2535,41 +2535,41 @@
       <c r="G38" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="H38" s="53" t="s">
+      <c r="H38" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="54"/>
-      <c r="L38" s="54"/>
-      <c r="M38" s="80"/>
+      <c r="I38" s="95"/>
+      <c r="J38" s="95"/>
+      <c r="K38" s="95"/>
+      <c r="L38" s="95"/>
+      <c r="M38" s="115"/>
     </row>
     <row r="41" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="71" t="s">
+      <c r="B42" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="72"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="71" t="s">
+      <c r="C42" s="57"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="72"/>
-      <c r="G42" s="73"/>
-      <c r="H42" s="71" t="s">
+      <c r="F42" s="57"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="73"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="58"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B43" s="86" t="s">
+      <c r="B43" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="87"/>
-      <c r="D43" s="88"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="105"/>
       <c r="E43" s="28">
         <v>1</v>
       </c>
@@ -2579,18 +2579,18 @@
       <c r="G43" s="30">
         <v>3</v>
       </c>
-      <c r="H43" s="86"/>
-      <c r="I43" s="87"/>
-      <c r="J43" s="87"/>
-      <c r="K43" s="87"/>
-      <c r="L43" s="88"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
+      <c r="L43" s="105"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B44" s="59" t="s">
+      <c r="B44" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="60"/>
-      <c r="D44" s="82"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="69"/>
       <c r="E44" s="47">
         <v>1</v>
       </c>
@@ -2600,20 +2600,20 @@
       <c r="G44" s="24">
         <v>4</v>
       </c>
-      <c r="H44" s="81" t="s">
+      <c r="H44" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="I44" s="60"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="60"/>
-      <c r="L44" s="82"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="69"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B45" s="59" t="s">
+      <c r="B45" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="60"/>
-      <c r="D45" s="82"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="47">
         <v>2</v>
       </c>
@@ -2623,20 +2623,20 @@
       <c r="G45" s="24">
         <v>0</v>
       </c>
-      <c r="H45" s="81" t="s">
-        <v>70</v>
-      </c>
-      <c r="I45" s="60"/>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60"/>
-      <c r="L45" s="82"/>
+      <c r="H45" s="116" t="s">
+        <v>120</v>
+      </c>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63"/>
+      <c r="K45" s="63"/>
+      <c r="L45" s="69"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B46" s="59" t="s">
+      <c r="B46" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="60"/>
-      <c r="D46" s="82"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="47">
         <v>8</v>
       </c>
@@ -2646,20 +2646,20 @@
       <c r="G46" s="24">
         <v>0</v>
       </c>
-      <c r="H46" s="81" t="s">
-        <v>72</v>
-      </c>
-      <c r="I46" s="60"/>
-      <c r="J46" s="60"/>
-      <c r="K46" s="60"/>
-      <c r="L46" s="82"/>
+      <c r="H46" s="116" t="s">
+        <v>71</v>
+      </c>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="69"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B47" s="59" t="s">
+      <c r="B47" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="60"/>
-      <c r="D47" s="82"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="69"/>
       <c r="E47" s="47">
         <v>4</v>
       </c>
@@ -2669,20 +2669,20 @@
       <c r="G47" s="24">
         <v>0</v>
       </c>
-      <c r="H47" s="81" t="s">
-        <v>71</v>
-      </c>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="82"/>
+      <c r="H47" s="116" t="s">
+        <v>70</v>
+      </c>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="69"/>
     </row>
     <row r="48" spans="2:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="53" t="s">
+      <c r="B48" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="54"/>
-      <c r="D48" s="80"/>
+      <c r="C48" s="95"/>
+      <c r="D48" s="115"/>
       <c r="E48" s="46">
         <v>6</v>
       </c>
@@ -2692,671 +2692,605 @@
       <c r="G48" s="23">
         <v>0</v>
       </c>
-      <c r="H48" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="80"/>
+      <c r="H48" s="128" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" s="95"/>
+      <c r="J48" s="95"/>
+      <c r="K48" s="95"/>
+      <c r="L48" s="115"/>
     </row>
     <row r="51" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="71" t="s">
+      <c r="B52" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="73"/>
-      <c r="E52" s="71" t="s">
+      <c r="C52" s="57"/>
+      <c r="D52" s="58"/>
+      <c r="E52" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F52" s="72"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="71" t="s">
+      <c r="F52" s="57"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="I52" s="72"/>
-      <c r="J52" s="72"/>
-      <c r="K52" s="72"/>
-      <c r="L52" s="73"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="58"/>
     </row>
     <row r="53" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B53" s="102" t="s">
-        <v>74</v>
-      </c>
-      <c r="C53" s="103"/>
-      <c r="D53" s="104"/>
+      <c r="B53" s="106" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" s="107"/>
+      <c r="D53" s="108"/>
       <c r="E53" s="31">
         <v>1</v>
       </c>
       <c r="F53" s="36"/>
       <c r="G53" s="37"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="87"/>
-      <c r="J53" s="87"/>
-      <c r="K53" s="87"/>
-      <c r="L53" s="88"/>
+      <c r="H53" s="127"/>
+      <c r="I53" s="60"/>
+      <c r="J53" s="60"/>
+      <c r="K53" s="60"/>
+      <c r="L53" s="105"/>
     </row>
     <row r="54" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B54" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="60"/>
-      <c r="D54" s="61"/>
+      <c r="B54" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64"/>
       <c r="E54" s="48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F54" s="34"/>
       <c r="G54" s="35"/>
-      <c r="H54" s="83" t="s">
-        <v>84</v>
-      </c>
-      <c r="I54" s="60"/>
-      <c r="J54" s="60"/>
-      <c r="K54" s="60"/>
-      <c r="L54" s="82"/>
+      <c r="H54" s="129" t="s">
+        <v>83</v>
+      </c>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
+      <c r="L54" s="69"/>
     </row>
     <row r="55" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B55" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="C55" s="60"/>
-      <c r="D55" s="61"/>
+      <c r="B55" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="63"/>
+      <c r="D55" s="64"/>
       <c r="E55" s="48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F55" s="34"/>
       <c r="G55" s="35"/>
-      <c r="H55" s="83" t="s">
-        <v>85</v>
-      </c>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="60"/>
-      <c r="L55" s="82"/>
+      <c r="H55" s="129" t="s">
+        <v>84</v>
+      </c>
+      <c r="I55" s="63"/>
+      <c r="J55" s="63"/>
+      <c r="K55" s="63"/>
+      <c r="L55" s="69"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B56" s="106" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" s="77"/>
-      <c r="D56" s="78"/>
+      <c r="B56" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="99"/>
+      <c r="D56" s="114"/>
       <c r="E56" s="48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F56" s="34"/>
       <c r="G56" s="35"/>
-      <c r="H56" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="I56" s="77"/>
-      <c r="J56" s="77"/>
-      <c r="K56" s="77"/>
-      <c r="L56" s="78"/>
+      <c r="H56" s="99" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" s="99"/>
+      <c r="J56" s="99"/>
+      <c r="K56" s="99"/>
+      <c r="L56" s="114"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B57" s="106" t="s">
-        <v>78</v>
-      </c>
-      <c r="C57" s="77"/>
-      <c r="D57" s="78"/>
+      <c r="B57" s="98" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" s="99"/>
+      <c r="D57" s="114"/>
       <c r="E57" s="48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F57" s="34"/>
       <c r="G57" s="35"/>
-      <c r="H57" s="77" t="s">
-        <v>87</v>
-      </c>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="78"/>
+      <c r="H57" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="I57" s="99"/>
+      <c r="J57" s="99"/>
+      <c r="K57" s="99"/>
+      <c r="L57" s="114"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B58" s="106" t="s">
-        <v>79</v>
-      </c>
-      <c r="C58" s="77"/>
-      <c r="D58" s="78"/>
+      <c r="B58" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="99"/>
+      <c r="D58" s="114"/>
       <c r="E58" s="48" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F58" s="34"/>
       <c r="G58" s="35"/>
-      <c r="H58" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="I58" s="77"/>
-      <c r="J58" s="77"/>
-      <c r="K58" s="77"/>
-      <c r="L58" s="78"/>
+      <c r="H58" s="99" t="s">
+        <v>113</v>
+      </c>
+      <c r="I58" s="99"/>
+      <c r="J58" s="99"/>
+      <c r="K58" s="99"/>
+      <c r="L58" s="114"/>
     </row>
     <row r="59" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="105"/>
-      <c r="C59" s="90"/>
-      <c r="D59" s="91"/>
+      <c r="B59" s="109"/>
+      <c r="C59" s="110"/>
+      <c r="D59" s="111"/>
       <c r="E59" s="32"/>
       <c r="F59" s="38"/>
       <c r="G59" s="39"/>
-      <c r="H59" s="90"/>
-      <c r="I59" s="90"/>
-      <c r="J59" s="90"/>
-      <c r="K59" s="90"/>
-      <c r="L59" s="91"/>
+      <c r="H59" s="110"/>
+      <c r="I59" s="110"/>
+      <c r="J59" s="110"/>
+      <c r="K59" s="110"/>
+      <c r="L59" s="111"/>
     </row>
     <row r="62" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="63" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="74" t="s">
+      <c r="B63" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="76"/>
-      <c r="E63" s="71" t="s">
+      <c r="C63" s="67"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F63" s="72"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="74" t="s">
+      <c r="F63" s="57"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="I63" s="75"/>
-      <c r="J63" s="75"/>
-      <c r="K63" s="75"/>
-      <c r="L63" s="76"/>
+      <c r="I63" s="67"/>
+      <c r="J63" s="67"/>
+      <c r="K63" s="67"/>
+      <c r="L63" s="68"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B64" s="101" t="s">
+      <c r="B64" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="C64" s="84"/>
-      <c r="D64" s="84"/>
+      <c r="C64" s="113"/>
+      <c r="D64" s="113"/>
       <c r="E64" s="31">
         <v>1</v>
       </c>
       <c r="F64" s="36"/>
       <c r="G64" s="37"/>
-      <c r="H64" s="84"/>
-      <c r="I64" s="84"/>
-      <c r="J64" s="84"/>
-      <c r="K64" s="84"/>
-      <c r="L64" s="85"/>
+      <c r="H64" s="113"/>
+      <c r="I64" s="113"/>
+      <c r="J64" s="113"/>
+      <c r="K64" s="113"/>
+      <c r="L64" s="126"/>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B65" s="59" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" s="60"/>
-      <c r="D65" s="61"/>
+      <c r="B65" s="62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="63"/>
+      <c r="D65" s="64"/>
       <c r="E65" s="49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F65" s="41"/>
       <c r="G65" s="42"/>
-      <c r="H65" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="I65" s="66"/>
-      <c r="J65" s="66"/>
-      <c r="K65" s="66"/>
-      <c r="L65" s="67"/>
+      <c r="H65" s="130" t="s">
+        <v>115</v>
+      </c>
+      <c r="I65" s="131"/>
+      <c r="J65" s="131"/>
+      <c r="K65" s="131"/>
+      <c r="L65" s="132"/>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B66" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="60"/>
-      <c r="D66" s="61"/>
+      <c r="B66" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="63"/>
+      <c r="D66" s="64"/>
       <c r="E66" s="50"/>
       <c r="F66" s="33"/>
       <c r="G66" s="33"/>
-      <c r="H66" s="68"/>
-      <c r="I66" s="69"/>
-      <c r="J66" s="69"/>
-      <c r="K66" s="69"/>
-      <c r="L66" s="70"/>
+      <c r="H66" s="136"/>
+      <c r="I66" s="137"/>
+      <c r="J66" s="137"/>
+      <c r="K66" s="137"/>
+      <c r="L66" s="138"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B67" s="59" t="s">
-        <v>90</v>
-      </c>
-      <c r="C67" s="60"/>
-      <c r="D67" s="61"/>
+      <c r="B67" s="62" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="63"/>
+      <c r="D67" s="64"/>
       <c r="E67" s="51"/>
       <c r="F67" s="33"/>
       <c r="G67" s="33"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="63"/>
-      <c r="J67" s="63"/>
-      <c r="K67" s="63"/>
-      <c r="L67" s="64"/>
+      <c r="H67" s="133"/>
+      <c r="I67" s="134"/>
+      <c r="J67" s="134"/>
+      <c r="K67" s="134"/>
+      <c r="L67" s="135"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B68" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="60"/>
-      <c r="D68" s="61"/>
+      <c r="B68" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="63"/>
+      <c r="D68" s="64"/>
       <c r="E68" s="51"/>
       <c r="F68" s="33"/>
       <c r="G68" s="33"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="63"/>
-      <c r="K68" s="63"/>
-      <c r="L68" s="64"/>
+      <c r="H68" s="133"/>
+      <c r="I68" s="134"/>
+      <c r="J68" s="134"/>
+      <c r="K68" s="134"/>
+      <c r="L68" s="135"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B69" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="C69" s="60"/>
-      <c r="D69" s="61"/>
+      <c r="B69" s="62" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="63"/>
+      <c r="D69" s="64"/>
       <c r="E69" s="51"/>
       <c r="F69" s="33"/>
       <c r="G69" s="33"/>
-      <c r="H69" s="62"/>
-      <c r="I69" s="63"/>
-      <c r="J69" s="63"/>
-      <c r="K69" s="63"/>
-      <c r="L69" s="64"/>
+      <c r="H69" s="133"/>
+      <c r="I69" s="134"/>
+      <c r="J69" s="134"/>
+      <c r="K69" s="134"/>
+      <c r="L69" s="135"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B70" s="59" t="s">
-        <v>93</v>
-      </c>
-      <c r="C70" s="60"/>
-      <c r="D70" s="61"/>
+      <c r="B70" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="63"/>
+      <c r="D70" s="64"/>
       <c r="E70" s="51"/>
       <c r="F70" s="33"/>
       <c r="G70" s="33"/>
-      <c r="H70" s="62"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="63"/>
-      <c r="K70" s="63"/>
-      <c r="L70" s="64"/>
+      <c r="H70" s="133"/>
+      <c r="I70" s="134"/>
+      <c r="J70" s="134"/>
+      <c r="K70" s="134"/>
+      <c r="L70" s="135"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B71" s="59" t="s">
-        <v>94</v>
-      </c>
-      <c r="C71" s="60"/>
-      <c r="D71" s="61"/>
+      <c r="B71" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="63"/>
+      <c r="D71" s="64"/>
       <c r="E71" s="51"/>
       <c r="F71" s="33"/>
       <c r="G71" s="33"/>
-      <c r="H71" s="62"/>
-      <c r="I71" s="63"/>
-      <c r="J71" s="63"/>
-      <c r="K71" s="63"/>
-      <c r="L71" s="64"/>
+      <c r="H71" s="133"/>
+      <c r="I71" s="134"/>
+      <c r="J71" s="134"/>
+      <c r="K71" s="134"/>
+      <c r="L71" s="135"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B72" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="C72" s="60"/>
-      <c r="D72" s="61"/>
+      <c r="B72" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="63"/>
+      <c r="D72" s="64"/>
       <c r="E72" s="51"/>
       <c r="F72" s="33"/>
       <c r="G72" s="33"/>
-      <c r="H72" s="62"/>
-      <c r="I72" s="63"/>
-      <c r="J72" s="63"/>
-      <c r="K72" s="63"/>
-      <c r="L72" s="64"/>
+      <c r="H72" s="133"/>
+      <c r="I72" s="134"/>
+      <c r="J72" s="134"/>
+      <c r="K72" s="134"/>
+      <c r="L72" s="135"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B73" s="59" t="s">
-        <v>96</v>
-      </c>
-      <c r="C73" s="60"/>
-      <c r="D73" s="61"/>
+      <c r="B73" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C73" s="63"/>
+      <c r="D73" s="64"/>
       <c r="E73" s="51"/>
       <c r="F73" s="33"/>
       <c r="G73" s="33"/>
-      <c r="H73" s="62"/>
-      <c r="I73" s="63"/>
-      <c r="J73" s="63"/>
-      <c r="K73" s="63"/>
-      <c r="L73" s="64"/>
+      <c r="H73" s="133"/>
+      <c r="I73" s="134"/>
+      <c r="J73" s="134"/>
+      <c r="K73" s="134"/>
+      <c r="L73" s="135"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B74" s="59" t="s">
-        <v>97</v>
-      </c>
-      <c r="C74" s="60"/>
-      <c r="D74" s="61"/>
+      <c r="B74" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C74" s="63"/>
+      <c r="D74" s="64"/>
       <c r="E74" s="51"/>
       <c r="F74" s="33"/>
       <c r="G74" s="33"/>
-      <c r="H74" s="62"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="63"/>
-      <c r="K74" s="63"/>
-      <c r="L74" s="64"/>
+      <c r="H74" s="133"/>
+      <c r="I74" s="134"/>
+      <c r="J74" s="134"/>
+      <c r="K74" s="134"/>
+      <c r="L74" s="135"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B75" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="C75" s="60"/>
-      <c r="D75" s="61"/>
+      <c r="B75" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75" s="63"/>
+      <c r="D75" s="64"/>
       <c r="E75" s="51"/>
       <c r="F75" s="33"/>
       <c r="G75" s="33"/>
-      <c r="H75" s="62"/>
-      <c r="I75" s="63"/>
-      <c r="J75" s="63"/>
-      <c r="K75" s="63"/>
-      <c r="L75" s="64"/>
+      <c r="H75" s="133"/>
+      <c r="I75" s="134"/>
+      <c r="J75" s="134"/>
+      <c r="K75" s="134"/>
+      <c r="L75" s="135"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B76" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="60"/>
-      <c r="D76" s="61"/>
+      <c r="B76" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" s="63"/>
+      <c r="D76" s="64"/>
       <c r="E76" s="51"/>
       <c r="F76" s="33"/>
       <c r="G76" s="33"/>
-      <c r="H76" s="62"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="63"/>
-      <c r="K76" s="63"/>
-      <c r="L76" s="64"/>
+      <c r="H76" s="133"/>
+      <c r="I76" s="134"/>
+      <c r="J76" s="134"/>
+      <c r="K76" s="134"/>
+      <c r="L76" s="135"/>
     </row>
     <row r="77" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B77" s="59" t="s">
-        <v>100</v>
-      </c>
-      <c r="C77" s="60"/>
-      <c r="D77" s="61"/>
+      <c r="B77" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="63"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="51"/>
       <c r="F77" s="33"/>
       <c r="G77" s="33"/>
-      <c r="H77" s="62"/>
-      <c r="I77" s="63"/>
-      <c r="J77" s="63"/>
-      <c r="K77" s="63"/>
-      <c r="L77" s="64"/>
+      <c r="H77" s="133"/>
+      <c r="I77" s="134"/>
+      <c r="J77" s="134"/>
+      <c r="K77" s="134"/>
+      <c r="L77" s="135"/>
     </row>
     <row r="78" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B78" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C78" s="60"/>
-      <c r="D78" s="61"/>
+      <c r="B78" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C78" s="63"/>
+      <c r="D78" s="64"/>
       <c r="E78" s="51"/>
       <c r="F78" s="33"/>
       <c r="G78" s="33"/>
-      <c r="H78" s="62"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="63"/>
-      <c r="K78" s="63"/>
-      <c r="L78" s="64"/>
+      <c r="H78" s="133"/>
+      <c r="I78" s="134"/>
+      <c r="J78" s="134"/>
+      <c r="K78" s="134"/>
+      <c r="L78" s="135"/>
     </row>
     <row r="79" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B79" s="59" t="s">
-        <v>102</v>
-      </c>
-      <c r="C79" s="60"/>
-      <c r="D79" s="61"/>
+      <c r="B79" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="63"/>
+      <c r="D79" s="64"/>
       <c r="E79" s="51"/>
       <c r="F79" s="33"/>
       <c r="G79" s="33"/>
-      <c r="H79" s="62"/>
-      <c r="I79" s="63"/>
-      <c r="J79" s="63"/>
-      <c r="K79" s="63"/>
-      <c r="L79" s="64"/>
+      <c r="H79" s="133"/>
+      <c r="I79" s="134"/>
+      <c r="J79" s="134"/>
+      <c r="K79" s="134"/>
+      <c r="L79" s="135"/>
     </row>
     <row r="80" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B80" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C80" s="60"/>
-      <c r="D80" s="61"/>
+      <c r="B80" s="62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C80" s="63"/>
+      <c r="D80" s="64"/>
       <c r="E80" s="51"/>
       <c r="F80" s="33"/>
       <c r="G80" s="33"/>
-      <c r="H80" s="62"/>
-      <c r="I80" s="63"/>
-      <c r="J80" s="63"/>
-      <c r="K80" s="63"/>
-      <c r="L80" s="64"/>
+      <c r="H80" s="133"/>
+      <c r="I80" s="134"/>
+      <c r="J80" s="134"/>
+      <c r="K80" s="134"/>
+      <c r="L80" s="135"/>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B81" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="C81" s="60"/>
-      <c r="D81" s="61"/>
+      <c r="B81" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="63"/>
+      <c r="D81" s="64"/>
       <c r="E81" s="51"/>
       <c r="F81" s="33"/>
       <c r="G81" s="33"/>
-      <c r="H81" s="62"/>
-      <c r="I81" s="63"/>
-      <c r="J81" s="63"/>
-      <c r="K81" s="63"/>
-      <c r="L81" s="64"/>
+      <c r="H81" s="133"/>
+      <c r="I81" s="134"/>
+      <c r="J81" s="134"/>
+      <c r="K81" s="134"/>
+      <c r="L81" s="135"/>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B82" s="59" t="s">
-        <v>105</v>
-      </c>
-      <c r="C82" s="60"/>
-      <c r="D82" s="61"/>
+      <c r="B82" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="63"/>
+      <c r="D82" s="64"/>
       <c r="E82" s="51"/>
       <c r="F82" s="33"/>
       <c r="G82" s="33"/>
-      <c r="H82" s="62"/>
-      <c r="I82" s="63"/>
-      <c r="J82" s="63"/>
-      <c r="K82" s="63"/>
-      <c r="L82" s="64"/>
+      <c r="H82" s="133"/>
+      <c r="I82" s="134"/>
+      <c r="J82" s="134"/>
+      <c r="K82" s="134"/>
+      <c r="L82" s="135"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B83" s="59" t="s">
-        <v>106</v>
-      </c>
-      <c r="C83" s="60"/>
-      <c r="D83" s="61"/>
+      <c r="B83" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="C83" s="63"/>
+      <c r="D83" s="64"/>
       <c r="E83" s="51"/>
       <c r="F83" s="33"/>
       <c r="G83" s="33"/>
-      <c r="H83" s="62"/>
-      <c r="I83" s="63"/>
-      <c r="J83" s="63"/>
-      <c r="K83" s="63"/>
-      <c r="L83" s="64"/>
+      <c r="H83" s="133"/>
+      <c r="I83" s="134"/>
+      <c r="J83" s="134"/>
+      <c r="K83" s="134"/>
+      <c r="L83" s="135"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B84" s="59" t="s">
-        <v>107</v>
-      </c>
-      <c r="C84" s="60"/>
-      <c r="D84" s="61"/>
+      <c r="B84" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="63"/>
+      <c r="D84" s="64"/>
       <c r="E84" s="51"/>
       <c r="F84" s="33"/>
       <c r="G84" s="33"/>
-      <c r="H84" s="62"/>
-      <c r="I84" s="63"/>
-      <c r="J84" s="63"/>
-      <c r="K84" s="63"/>
-      <c r="L84" s="64"/>
+      <c r="H84" s="133"/>
+      <c r="I84" s="134"/>
+      <c r="J84" s="134"/>
+      <c r="K84" s="134"/>
+      <c r="L84" s="135"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B85" s="59" t="s">
-        <v>108</v>
-      </c>
-      <c r="C85" s="60"/>
-      <c r="D85" s="61"/>
+      <c r="B85" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" s="63"/>
+      <c r="D85" s="64"/>
       <c r="E85" s="51"/>
       <c r="F85" s="33"/>
       <c r="G85" s="33"/>
-      <c r="H85" s="62"/>
-      <c r="I85" s="63"/>
-      <c r="J85" s="63"/>
-      <c r="K85" s="63"/>
-      <c r="L85" s="64"/>
+      <c r="H85" s="133"/>
+      <c r="I85" s="134"/>
+      <c r="J85" s="134"/>
+      <c r="K85" s="134"/>
+      <c r="L85" s="135"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B86" s="59" t="s">
-        <v>109</v>
-      </c>
-      <c r="C86" s="60"/>
-      <c r="D86" s="61"/>
+      <c r="B86" s="62" t="s">
+        <v>108</v>
+      </c>
+      <c r="C86" s="63"/>
+      <c r="D86" s="64"/>
       <c r="E86" s="51"/>
       <c r="F86" s="33"/>
       <c r="G86" s="33"/>
-      <c r="H86" s="62"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="63"/>
-      <c r="K86" s="63"/>
-      <c r="L86" s="64"/>
+      <c r="H86" s="133"/>
+      <c r="I86" s="134"/>
+      <c r="J86" s="134"/>
+      <c r="K86" s="134"/>
+      <c r="L86" s="135"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B87" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="C87" s="60"/>
-      <c r="D87" s="61"/>
+      <c r="B87" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="C87" s="63"/>
+      <c r="D87" s="64"/>
       <c r="E87" s="51"/>
       <c r="F87" s="33"/>
       <c r="G87" s="33"/>
-      <c r="H87" s="62"/>
-      <c r="I87" s="63"/>
-      <c r="J87" s="63"/>
-      <c r="K87" s="63"/>
-      <c r="L87" s="64"/>
+      <c r="H87" s="133"/>
+      <c r="I87" s="134"/>
+      <c r="J87" s="134"/>
+      <c r="K87" s="134"/>
+      <c r="L87" s="135"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B88" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="C88" s="60"/>
-      <c r="D88" s="61"/>
+      <c r="B88" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="63"/>
+      <c r="D88" s="64"/>
       <c r="E88" s="51"/>
       <c r="F88" s="33"/>
       <c r="G88" s="33"/>
-      <c r="H88" s="62"/>
-      <c r="I88" s="63"/>
-      <c r="J88" s="63"/>
-      <c r="K88" s="63"/>
-      <c r="L88" s="64"/>
+      <c r="H88" s="133"/>
+      <c r="I88" s="134"/>
+      <c r="J88" s="134"/>
+      <c r="K88" s="134"/>
+      <c r="L88" s="135"/>
     </row>
     <row r="89" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="C89" s="54"/>
-      <c r="D89" s="55"/>
+      <c r="B89" s="94" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89" s="95"/>
+      <c r="D89" s="97"/>
       <c r="E89" s="52"/>
       <c r="F89" s="40"/>
       <c r="G89" s="40"/>
-      <c r="H89" s="56"/>
-      <c r="I89" s="57"/>
-      <c r="J89" s="57"/>
-      <c r="K89" s="57"/>
-      <c r="L89" s="58"/>
+      <c r="H89" s="139"/>
+      <c r="I89" s="140"/>
+      <c r="J89" s="140"/>
+      <c r="K89" s="140"/>
+      <c r="L89" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="144">
-    <mergeCell ref="B4:P4"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="N7:Q9"/>
-    <mergeCell ref="N11:Q14"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:L42"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:L44"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H25:L25"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="H20:L20"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="H23:L23"/>
-    <mergeCell ref="H24:L24"/>
-    <mergeCell ref="H36:M36"/>
-    <mergeCell ref="H38:M38"/>
-    <mergeCell ref="H64:L64"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="H34:M34"/>
-    <mergeCell ref="H35:M35"/>
-    <mergeCell ref="H37:M37"/>
-    <mergeCell ref="H53:L53"/>
-    <mergeCell ref="H59:L59"/>
-    <mergeCell ref="H46:L46"/>
-    <mergeCell ref="H47:L47"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="H63:L63"/>
-    <mergeCell ref="H56:L56"/>
-    <mergeCell ref="H57:L57"/>
-    <mergeCell ref="H58:L58"/>
-    <mergeCell ref="H48:L48"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="H52:L52"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="H54:L54"/>
-    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="H89:L89"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="H86:L86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="H87:L87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="H88:L88"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="H83:L83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="H84:L84"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="H85:L85"/>
+    <mergeCell ref="H76:L76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="H77:L77"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="H81:L81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="H82:L82"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="H79:L79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="H80:L80"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="H78:L78"/>
+    <mergeCell ref="B76:D76"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="H65:L65"/>
     <mergeCell ref="B71:D71"/>
@@ -3379,34 +3313,100 @@
     <mergeCell ref="H67:L67"/>
     <mergeCell ref="B70:D70"/>
     <mergeCell ref="H70:L70"/>
-    <mergeCell ref="H76:L76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="H77:L77"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="H81:L81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="H82:L82"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="H79:L79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="H80:L80"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="H78:L78"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="H89:L89"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="H86:L86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="H87:L87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="H88:L88"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="H83:L83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="H84:L84"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="H85:L85"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="H63:L63"/>
+    <mergeCell ref="H56:L56"/>
+    <mergeCell ref="H57:L57"/>
+    <mergeCell ref="H58:L58"/>
+    <mergeCell ref="H48:L48"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="H52:L52"/>
+    <mergeCell ref="H45:L45"/>
+    <mergeCell ref="H54:L54"/>
+    <mergeCell ref="H55:L55"/>
+    <mergeCell ref="H64:L64"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="H34:M34"/>
+    <mergeCell ref="H35:M35"/>
+    <mergeCell ref="H37:M37"/>
+    <mergeCell ref="H53:L53"/>
+    <mergeCell ref="H59:L59"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="H47:L47"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:L42"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:L44"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="H12:L12"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H25:L25"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H20:L20"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="H23:L23"/>
+    <mergeCell ref="H24:L24"/>
+    <mergeCell ref="H36:M36"/>
+    <mergeCell ref="H38:M38"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B4:P4"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="N7:Q9"/>
+    <mergeCell ref="N11:Q14"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>